<commit_message>
Added results for R4-computer-game1 model
</commit_message>
<xml_diff>
--- a/results/correct models/R4-computer-game1/associations_contradiction_check.xlsx
+++ b/results/correct models/R4-computer-game1/associations_contradiction_check.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,1614 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>It costs the player a single move to enter the atmosphere from the adjacent cell.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A entry point is adjacent to cells </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Statement 2 speculates that it will cost the player a single move to enter the atmosphere from the adjacent cell. This implies that there is a relationship between the entry point and the cell, and that this relationship involves a single cell as the player is only using a single move. Presumably, a single move corresponds to a single cell. Therefore, the multiplicity from entry point to cell in this statement would be 1 (one).
+On the other hand, Statement 1 specifies that an instance of type entry point is associated with many instances of type cell, which denotes a multiplicity greater than 1.
+Even though both statements establish a relationship between the entry point and the cells, the multiplicity inferred from each statement differs.
+Conclusion: Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>If an announced hypothesis is incorrect, the player loses the game and cannot pose hypotheses any longer or make moves on the board but must continue refuting the hypotheses of other players.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Statement 2 says that if a player announces an incorrect hypothesis, they lose the ability to make legal moves. So, it indicates that under certain conditions (an incorrect hypothesis), an instance of type player is associated with no instances of type legal move. This multiplicity indeed differs from that described in statement 1, where it is stated that a player is associated with many instances of type legal move.
+Conclusion: Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Other players are informed that the hypothesis was refuted but need to be shown the piece of evidence that refuted the hypothesis.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have hypothesis </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Statement 2 indicates that "Other players are informed that the hypothesis was refuted but need to be shown the piece of evidence that refuted the hypothesis." This suggests an association between the players and the hypothesis as players are informed about the status of a hypothesis. 
+However, the multiplicity is not clearly stated in statement 2. It does not specify whether each player is associated with one or multiple hypotheses. Thus, we cannot definitively say if multiplicity of the association inferred from statement 2 is the same or different from the multiplicity described in statement 1.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>The questions form a hypothesis for the murder circumstance and perpetrator, which the remaining players are invited to disprove with their evidence.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A question is asked by a player</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Statement 2 describes that the questions, collectively, culminate into forming a hypothesis. These questions are then used by the remaining players to disprove the murder circumstance and perpetrator. However, unlike statement 1, this does not clearly describe a direct association between a single question and a single player. Instead, it seems to suggest a many-to-many relationship, where multiple questions can be involved with multiple players. 
+But given the lack of explicit declaration of a connection between a single question and a single player, a definitive multiplicity cannot be determined in statement 2.
+Conclusion:Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>The planets, Linuta and Verlute, have a wormhole connecting each other, as do Earth and Evilon.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Analyzing statement 2, it mentions that there are specific pairs of planets (Linuta and Verlute, Earth and Evilon) that have a wormhole connecting each other. This implies that a given planet (from the pairs mentioned) is only associated with one other specific planet.
+In contrast, statement 1 states that a planet is associated with many planets, which implies multiplicity in the relationships from one planet to other planets.
+Based on this analysis, it can be observed that the multiplicity of relationships differs between statement 1 and statement 2. While the first mentions a one-to-many relationship, the second suggests specific one-to-one relationships between planets.
+Conclusion: Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A player visits a planet by making legal moves on the board until a cell adjacent to an atmosphere entry point is reached.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>In statement 2, a "player visits a planet", which suggests an association between a player and a planet. However, the association between different instances of planets is not explicitly stated or described. The player visits a planet by “making legal moves until a cell adjacent to an atmosphere entry point is reached". The context implies that the player can visit different planets. However, the specific multiplicity from one planet to another is not clear from the text. We can thus determine that statement 2 does not provide enough information to conclude anything about the multiplicity relationship from planet to planet.
+Conclusion:Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A player whose token resides on one of four planets having wormhole connections to other planets may choose not to spin the spinner and take the wormhole directly to the other planet.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Statement 2 mentions "one of four planets having wormhole connections to other planets." This indicates that a planet (where the player's token resides) may be associated with one to four planets (as it specifies one of four). However, the other ends of these wormholes could potentially lead to the same planet or different ones.
+The multiplicity in this case is said to range from one to four (1...4). This means that one planet can be associated with up to four other planets. 
+On the other hand, Statement 1 describes a scenario where a single planet can have a wormhole to multiple planets, implying a multiplicity of one to many (1...*). It does not limit the number of associated planets to just four. 
+So even though both statements point to a multiplicity where one planet can be connected to more than one planet through wormholes, the range of this connection, the multiplicity, seems to differ between the two statements.
+Conclusion: Yes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The objective of player movement throughout the universe is to investigate specific planets to determine if that was the murder site.</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests that the player is moving throughout the universe to investigate specific planets. However, it does not clarify if the player needs a separate hypothesis for each planet they explore or if each player explores multiple planets under a single hypothesis. Therefore, the exact relationship between a hypothesis and the planets -whether one-to-one, one-to-many, or many-to-one- is not explicitly mentioned in statement 2.
+So, the multiplicity between hypothesis and planet in statement 2 cannot be accurately determined. It could be one-to-one, one-to-many, or many-to-one. We do not have enough information to confirm or deny if it is the same as or different from the 'one-to-one' multiplicity mentioned in statement 1.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A player visits a planet by making legal moves on the board until a cell adjacent to an atmosphere entry point is reached.</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A entry point is adjacent to cells </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>In Statement 2, the player is said to reach "a cell adjacent to an atmosphere entry point," which implies that there could be many cells, but the player only needs to reach one. This implies an association of one entry point to many cells. 
+This multiplicity mirrors the multiplicity from Statement 1 which also describes a one-to-many relationship between an entry-point and its adjacent cells. 
+Therefore, 
+Conclusion: No. The multiplicity from the entry point to the cell in Statement 2 does not differ from that described in Statement 1.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Also, a player may not move into a cell occupied by another player's token.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A entry point is adjacent to cells </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The multiplicity in statements 1 and 2 are referring to two different associations. In statement 1, multiplicity is about the relationship between the entry point and cell. In other words, it is outlining that a single entry point may be adjacent to many cells. 
+In statement 2, the multiplicity is about the relationship between a player and a cell. Specifically, it elucidates that a player may not move into a cell occupied by another player's token. It neither specifically mentions nor implies any association between the entry point and the cell.
+As a result, the multiplicity of the entry point to the cell in statement 2 cannot be determined. Therefore, we cannot compare it to the multiplicity outlined in statement 1.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>The player may change directions multiple times but cannot enter the same cell twice during a single turn.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A entry point is adjacent to cells </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>The second statement explains how the player interacts with the cells, specifically that the player cannot enter the same cell twice during a single turn. This statement, however, does not elaborate on how the entry point is associated with the cells. While the statement implies a relationship between the entry point and cells in the sense that the player moves from the entry point, it does not illustrate if one entry point can be adjacent to many cells (as in the first statement) or if its associated with just one. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>It costs the player a single move to enter the atmosphere from the adjacent cell.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>A legal move is from a cell</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Statement 2 indicates that a player must execute a legal move to transition from an adjacent cell to enter the atmosphere. This implies that a legal move could possibly be associated with more than one cell i.e., the cell the player is currently located in and the adjacent cell towards the atmosphere. However, the statement does not explicitly describe whether the same legal move or different legal moves are executed for each cell. 
+Therefore, it can't be verified with certainty how the multiplicity of a cell to the legal move is affected based on statement 2.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>It costs the player a single move to enter the atmosphere from the adjacent cell.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A legal move has a a to which is a cell</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Statement 2 implies that a player can move from one cell (adjacent cell) to another (atmosphere) with a single legal move. This implies that a legal move can still be associated with one cell, the destination cell. However, it is not clear from this statement whether each legal move is always associated with only one cell or whether a legal move could potentially involve multiple cells (for example, if the game rules allowed for a 'jump' move that skips over intermediate cells). Therefore, while there could be an association between a legal move and a cell in statement 2, it does not provide enough specifics about the exact nature or details of this alleged relationship. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The murder hypothesis is communicated to all players.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Statement 2 does not provide any information regarding the association between a player and legal moves. It only mentions that the murder hypothesis is communicated to all players. Therefore, there's not enough information to determine the multiplicity from player to the legal move.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>The wormholes connect certain planets.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Statement 2 speaks about wormholes and planets, both of which have no clear relationship or association with the player and legal move entities mentioned in statement 1. Even if one were to draw indirect associations (such as a wormhole possibly being a legal move for a player), the specific multiplicity of these potential connections is not outlined in statement 2.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>In contrast, the server coordinates communication between players and orchestrates the sequence of events of the game.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Statement 2 primarily discusses the role of the "server" in coordinating communication and orchestrating the game sequence. It does mention players, but there's no clear information or indication about how the server, players, and legal moves relate to each other. There's no stated association between players and legal moves in this context.
+Given that we are trying to determine if the multiplicity of 'player' to 'legal move' described in statement 1 differs from that in statement 2, but statement 2 does not provide any relevant information to make this comparison, it is difficult to form a definite conclusion.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>These entry points are graphically depicted on the game as a diagonal line off a square on the board leading into a planet's atmosphere.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Statement 2 discusses the graphical depiction of entry points in the game, particularly how they relate to a square on the board and a planet's atmosphere. There is no direct reference or association to a player or their legal moves. Because of this, it is impossible to determine any kind of multiplicity from a player to a legal move based on this statement. Therefore, we cannot compare it with the multiplicity given in statement 1. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>A legal move consists of a player moving their token, the number of moves determined by the spinner, either horizontally or vertically, but not diagonally.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Statement 2 describes the components and limitations of a "legal move." It specifically indicates that a legal move is tied to a single player moving their token in a specific way. While it provides more context about what a legal move is, it does not explicitly change or contradict the multiplicity outlined in statement 1. The first statement indicates that "a player can have legal moves," which allows for multiple legal moves for a single player, and the second statement does not specify any different association.
+Conclusion: No</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The questions form a hypothesis for the murder circumstance and perpetrator, which the remaining players are invited to disprove with their evidence.</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Statement 2 says "The questions form a hypothesis for the murder circumstance and perpetrator, which the remaining players are invited to disprove with their evidence." The statement does not provide any details about the relationship between players and legal moves. It talks about players disproving a hypothesis with their evidence, which doesn't necessarily equate to a legal move. It also doesn't provide any details about the multiplicity, i.e., how many legal moves a player might have. 
+Therefore, we cannot determine if the multiplicity is the same or different from the one in statement 1 that a player can have many legal moves.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Players may also travel through a few strategically placed wormholes.</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests a player may travel through wormholes, which implies a possible association with another type of move, specifically a "wormhole move." However, it does not explicitly state that these wormhole travels are considered "legal moves" or directly relate to 'legal moves'. 
+Therefore, it is unclear if this would affect or alter the multiplicity between a player and a legal move as stated in statement 1. We are unable to definitively determine the multiplicity from player to legal move based on the information provided in statement 2 alone.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Also, a player may not move into a cell occupied by another player's token.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a condition that limits the possible number of legal moves a player can have. Specifically, it limits the legal moves to cells not occupied by another player's token. However, it does not specify the exact number or range of legal moves a player can have, and thus doesn't provide a clear multiplicity from player to legal move. So even though it appears that the legal moves might be different due to the condition presented in statement 2, we don't have enough information to be certain. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>As the players travel through the universe, they are permitted to ask questions about what information their fellow players possess.</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Statement 2 has nothing to do with the multiplicity from player to legal move. It rather represents an association between players, allowing them to communicate and request information. The mentioned players in the statement are not directly related to their legal moves. Thus, it becomes uncertain if the multiplicity from player to legal move differs, is the same, or even exists pertaining to statement 2. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>The game is an intergalactic murder mystery, which emulates a board game scenario in which players spin a wheel to determine a randomly selected number of moves by which they travel through space to various planets.</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Statement 2 provides a description of the game which involves players making moves determined by spinning a wheel. However, the statement does not specify if these moves are 'legal moves' or give a specific quantity of 'legal moves' a player could have. The multiplicity described in statement 1 is a player having many instances of a 'legal move'. Based on statement 2, it is unclear if this multiplicity is the same or different because 'legal move' is not explicitly mentioned in relation to the player.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Other players are informed that the hypothesis was refuted but need to be shown the piece of evidence that refuted the hypothesis.</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Statement 2 does not provide any explicit information about an association between a player and legal moves. It simply discusses a hypothesis being refuted, other players being informed, and the need for them to be shown evidence. However, it doesn't mention if a player can have many legal moves, one legal move or any at all.
+By analyzing Statement 2, we can therefore ascertain that there isn't enough detailed information to establish the multiplicity from the player to the legal move. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>The first player to accomplish this wins the game.</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a condition for winning the game - being the first player to accomplish a certain task. However, this statement does not provide information about the relationship between a player and their legal moves. It merely discusses a condition of the game's outcome. Therefore, we cannot determine the multiplicity from player to the legal move based on Statement 2.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>A player whose token resides on one of four planets having wormhole connections to other planets may choose not to spin the spinner and take the wormhole directly to the other planet.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>The statement 2 specifies a more particular situation where the player, under a certain condition—residing on one of the four planets, can choose to make a legal move, either to spin the spinner or use the wormhole. However, statement 2 doesn't specifically address how many legal moves a player could have under this situation. It technically suggests at least two potential legal moves (spinning the spinner or using the wormhole), but it doesn't limit the moves to only these two or provide information how many other legal moves a player could make while in this context. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>If a player draws an incorrect conclusion, they lose the game.</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Statement 2 focuses on the consequences a player faces in the event they draw an incorrect conclusion, leading to them losing the game. It does not provide specific information about the multiplicity of associations between a player and legal moves. It doesn't describe whether a player has one or multiple legal moves available, nor does it contradict the assertion from Statement 1 that a player can have multiple legal moves. 
+Based on this, conclusion would be:
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>The solution is then broadcast to all players.</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Statement 2 implies that multiple instances of players are associated with the solution; however, it does not discuss any association between players and legal moves specifically. This statement does not provide a clear correlation or ratio nor does it clarify whether every player has multiple legal moves or only one.
+Thus, there is not enough information provided in statement 2 to determine the multiplicity of the association between a player and a legal move, or how it compares to the multiplicity described in statement 1. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>The game's objective is to gather clues while traveling about the universe.</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Statement 2 provides information about the objective of the game, which is to gather clues while traveling through the universe. However, it does not mention anything about the players' association with the legal moves, nor does it give any specific number of legal moves associated with a player.
+Therefore, we can't determine the multiplicity of the relationship between player and legal move from statement 2. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>This element is primarily dictated by luck since the wheel's spin determines the speed at which a player reaches a destination.</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Statement 2 primarily discusses the role of luck in determining the speed at which a player reaches a destination. The notion of a player's legal moves does not seem to directly factor into this context. It does not give any information regarding the association between a player and legal moves, nor does it provide any hints about the multiplicity of such an association, if it exists.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>The player is considered to be on the planet as soon as the planet's atmosphere has been entered.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests that a player is associated with a planet once they enter its atmosphere. However, this statement does not provide any direct information about how a player is associated with legal moves in this context. 
+Without any explicit mention of an association between player and legal moves within this statement, it is impossible to determine the multiplicity of that relationship within the context of statement 2. Therefore, we cannot accurately compare the multiplicity described in statement 2 to that of statement 1. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>A player may not re-visit the same planet on a single turn.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests that a player has a constraint on their legal moves -- i.e., they cannot revisit the same planet on a single turn. This suggests that while multiple legal moves are possible, they are restricted by the condition of not revisiting the same planet. 
+However, the specific multiplicity of legal move instances associated with each player instance isn't directly indicative from this statement. Therefore, it could be interpreted that the multiplicity could potentially be the same, less, or even greater than in statement 1, depending on additional factors not provided here.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>The player may change directions multiple times but cannot enter the same cell twice during a single turn.</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests that a player can change directions multiple times which implies numerous legal moves per turn, but the limitation of not entering the same cell twice during the turn indicates a restriction on these moves. This gives us a hint towards a large but constrained number of associations between the player instance and instances of type legal move.
+However, it might not necessarily alter the multiplicity mentioned in Statement 1 that a player can have many legal moves. Statement 1 does not specify the conditions of these moves as being in a single turn or across multiple turns. The many legal moves a player can have could be considered over a span of entire gameplay and not just a single turn.
+Conclusion: No. The multiplicity in Statement 2 does not explicitly differ from the one described in Statement 1. However, it's important to note that Statement 2 seems to provide additional conditionality to the movements of player not clear in statement 1.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Each player receives information concerning the murder, and no players receive the same information.</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Statement 2 describes the relationship between a player and the information they receive concerning the murder. However, it does not specify any relationship between a player and legal moves. Therefore, we cannot determine if there is any multiplicity between player and legal move based on the information given in statement 2.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>A player wins the game by announcing their murder hypothesis, consisting of a planet, a perpetrator, and a murder weapon at any time during their turn, and having the server determine that the hypothesis is correct.</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a specific scenario of how a player can win the game. It illustrates one type of legal move a player can make i.e., announcing their murder hypothesis and having it be determined correct by the server. However, the statement doesn't explicitly clarify if a player can make many such moves or just a single one, nor does it clarify if there are other types of legal moves available to the player.
+Therefore, based on the information provided in statement 2, we cannot definitively determine the multiplicity of the relationship between the player and legal moves. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>The planets, Linuta and Verlute, have a wormhole connecting each other, as do Earth and Evilon.</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>The second statement (statement 2) makes no mention of a player or legal moves. The focus of statement 2 is on planets and their wormholes, not on game players which are the focus of statement 1. Therefore, it doesn't provide any context or information that allows us to determine the multiplicity of players and legal moves. We cannot say whether the multiplicity mentioned in statement 2 differs from statement 1 because these concepts are not addressed in statement 2.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>To visit a planet, a player must enter the planet's atmosphere at one of the predefined entry points.</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests that in order for a player to enter a planet's atmosphere, there must be at least one predefined entry point that's considered as a legal move. Since the predefined entry points are referred as the legal moves a player can make, it implies that a player is still associated with many legal moves, it's just that the action of entering a planet’s atmosphere restricts the player to one legal move at a time.
+As per the given scenario, there may be multiple predefined entry points (legal moves), but a player can only choose one at a time to enter a planet’s atmosphere. Therefore, the multiplicity from player to the legal move in the context of statement 2 could be considered as 'one to many'; a player can have many legal moves (entry points), but selects one to execute at a time.
+This multiplicity seems similar to the one described in Statement 1 where a player is associated with many instances of legal moves. 
+Therefore:
+Conclusion: No, the multiplicity described in Statement 2 does not differ from the one stated in Statement 1.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Each planet has between one and three predefined atmospheric entry points.</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Statement 2 does not mention or depict any relation between a player and legal moves. The statement is about the association of planets with predefined atmospheric entry points which is an entirely different subject matter. Therefore, it doesn't provide any information to determine or change the multiplicity from player to the legal move that is described in statement 1.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>This application will, therefore, take on a client/server structure where each client supports one player's view of the game.</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Statement 2 discusses the structure of a game application, mentioning that each client supports one player's view of the game. It, however, does not provide specific information about how many legal moves a player can have in this scenario.
+The multiplicity between player and legal move in statement 1 is 'one-to-many' as it indicates that one player is associated with many legal moves. But statement 2 does not give explicit information about the multiplicity between player and legal move.
+Therefore, the conclusion is:
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>The game's strategy is embodied in selecting questions to ask other players, selecting planet destinations, and efficiently deducing the correct murder scenario.</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Analyzing statement 2, it's described that a strategy in this game involves players selecting questions to ask other players, choosing planet destinations, and working to deduce the correct murder scenario. Yet, we also notice that there isn't any explicit mention of 'legal moves' or any clear link of the players to 'legal moves' in statement 2. 
+The multiplicity, that is, the associations between the player and the 'legal move' cannot be identified from statement 2, as there is no explicit connection or link given between a player to a legal move. 
+Considering these points, the term 'legal moves' is only generalized in the context of players in statement 1, while it has not been detailed or mentioned in statement 2.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>The goal of the class project is to implement an Internet-based, who-done-it-style game called Galaxy Sleuth.</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Statement 2 describes the goal of a class project and gives information about what type of game is to be implemented. However, it doesn't give any specific details about the relationship between a player and legal moves within the Galaxy Sleuth game. 
+Therefore, we do not have enough information to determine the multiplicity from player to legal move in the context described by statement 2. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>When the correct hypothesis is announced, all players are informed of the circumstances of the murder.</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a situation where all players are informed when the correct hypothesis is announced. However, the statement does not provide any details about the relation between a player and the legal moves. It only mentions that players receive certain information, not that they perform legal moves or are associated with them. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>After gathering a certain set of clues and applying deductive reasoning, players may deduce the perpetrator and circumstance of the murder.</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Statement 2 implies that a player, through gathering clues and using deductive reasoning, may deduce the circumstances behind the murder. This process, which likely involves multiple steps, can be interpreted as multiple legal moves. Therefore, the multiplicity from player to legal move in statement 2 can be viewed as 'many', as a player will likely have to make many legal moves (gathering clues, deducing, etc.) to identify the perpetrator.
+That being said, the statement 2 does not explicitly mention or describe the association between the player and the legal moves. It does insinuate an indirect relationship as the process of deduction can be associated with legal moves, but it does not directly outline this connection.
+Therefore, while we can infer a potential multiplicity, the lack of explicit, definable relation means we cannot firmly determine if the multiplicity is the same as in statement 1 or different.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>A player visits a planet by making legal moves on the board until a cell adjacent to an atmosphere entry point is reached.</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a process that involves a player making multiple legal moves until a certain condition is met, i.e reaching a cell adjacent to an atmosphere entry point on a planet. This means that a player can be associated with multiple instances of legal moves. Therefore, the multiplicity from player to legal move here also can be described as "one to many".
+However, statement 2 does not provide information on any limitations or specifics in terms of how many legal moves a player can make. This might suggest a potentially infinite amount of possible legal moves associated with a player. 
+Considering the information given in statement 1 and 2, it seems that both statements indicate a "one to many" relationship between a player and legal moves.
+Conclusion: No, the multiplicity in statement 2 does not seem to differ from the one described in statement 1 as both show a "one to many" relationship.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>The player can enter the planet's atmosphere in a different number of moves.</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests that a player has an associated number of moves (which could be legal moves). It implies a potential variety in the number of moves or steps to enter the planet's atmosphere, which does align with the notion mentioned in the first statement that a player can have multiple legal moves. However, even though it implies association, it does not explicitly specify the nature of that association, hence does not solidify the "one to many" relationship.
+In other words, statement 2 does not provide enough evidence to clearly determine whether the multiplicity from player to legal move is different or the same from statement 1, as it does not explicitly mention "legal moves" and does not provide concrete information about the number of moves. We can assume each different number of moves could be a legal move, but it is an assumption rather than a fact based on the statement.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>The game is Internet-based in that players can play each other from remote sites on the Internet.</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Statement 2 does not give any information regarding the association between a player and legal moves in the game. It talks about the game being internet-based and that players can play with each other remotely. Unless we know that the internet-based nature of the game influences the number of legal moves a player can make, we can't determine the multiplicity from player to legal move from this statement. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>If the hypothesis cannot be denied, all players are informed of that fact.</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Statement 2 mentions that "all players are informed of that fact" but it does not provide any detailed information about the association from players to legal moves. It emphasizes on the communication between some sender (not defined) and all players but it does not explicitly mention anything about 'legal move' in its context. 
+Therefore, there is not enough information to determine the multiplicity from player to legal move based on statement 2.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>It costs the player a single move to enter the atmosphere from the adjacent cell.</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Statement 2 specifies that it costs a player a single move to enter the atmosphere from the adjacent cell. In this context, this statement implies that an instance of type player is associated with only one instance of a legal move at a time (due to the phrase "a single move"). This suggests a multiplicity of 1 from player to legal move.
+Statement 1, on the other hand, allows for multiple instances of type legal move to be associated with a player. This implies a multiplicity of many from player to legal move.
+Hence, the multiplicity as described in statement 2 (1:1) does differ from that in statement 1 (1:many).
+Conclusion: Yes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>If a player can disprove the hypothesis, that information is communicated only to the inquiring player.</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Statement 2 speaks about a potential association of a player with disproving a hypothesis. This information is then communicated to the inquiring player. However, it doesn't include any specific information about the association between a player and a legal move. Therefore, the statement does not provide enough information to determine a multiplicity from player to legal move.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>The objective of player movement throughout the universe is to investigate specific planets to determine if that was the murder site.</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Statement 2 does not provide a direct association between a player and a legal move. It discusses the objective of player movement throughout the universe and the purpose behind it, but it does not specify whether these movements are considered as "legal moves", nor does it indicate how many legal moves a player might have.
+In comparison, statement 1 clearly indicates that a player is associated with many instances of legal move. There are no equivalent instances of legal moves for a player mentioned in statement 2. Furthermore, statement 1 infers a potentially limitless number of legal moves per player while statement 2 does not specify the number of times a player can move.
+Due to these reasons, we can't determine the multiplicity from player to legal move in statement 2 because it does not provide enough details.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Part of the game, therefore, involves reaching suspicious locations quickly to investigate them.</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have legal moves </t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>The second statement does not directly describe the relationship between a player and legal moves. The line, "Part of the game, therefore, involves reaching suspicious locations quickly to investigate them," is more about the objectives of the game instead of the relationship between players and their moves. While it can be conjectured that reaching suspicious locations quickly could involve many legal moves, it is still not expressly stated. Hence, this statement does not provide definite information regarding the multiplicity from players to legal moves.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>The game's objective is to gather clues while traveling about the universe.</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>A player can have gathereds which are clues</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Statement 2 implies that a player is likely to gather multiple clues while traveling about the universe, which assumes that a player is associated with many clues. Therefore, the multiplicity from player to clue in statement 2 is 'one to many' or '1:n'. 
+This is similar to the multiplicity in statement 1 where a player can have many gathered clues meaning an instance of type player can be associated with many instances of type clue. 
+Conclusion: No.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>After gathering a certain set of clues and applying deductive reasoning, players may deduce the perpetrator and circumstance of the murder.</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>A player can have gathereds which are clues</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Statement 2 implies that a player gathers clues to piece together information about the murder. Just like in statement 1, this similarly indicates an association between the player and clues. However, statement 2 does not specify the exact number of clues a player can gather, but the context implies that multiple clues are gathered to deduce the information, not just one. 
+Statement 1 clearly states that there are multiple clues associated with a single player – this association in statement 2 is similarly implied. Both statements imply that an instance of type player is associated with multiple instances of type clue.
+Conclusion: No</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>The game's objective is to gather clues while traveling about the universe.</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>A clue has player</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Statement 2 does not explicitly mention any direct association between a clue and a player. However, it implies that a player (while in the process of playing the game) could gather multiple clues. This suggests that multiple instances of type clue could be associated with an instance of type player. This implies a multiplicity connection where one player could be associated with multiple clues. 
+This description seems to suggest a different multiplicity compared to Statement 1 which insists that an instance of type clue is associated with exactly one instance of type player. Therefore, based on available information;
+Conclusion: Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>After gathering a certain set of clues and applying deductive reasoning, players may deduce the perpetrator and circumstance of the murder.</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>A clue has player</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>From the analysis of Statement 2, it can be inferred that multiple clues could be associated with a player to deduce the perpetrator and circumstance of the murder. This implies that a clue is not linked to exactly one player but likely several for them to compile and solve the mystery. However, it is impossible to definitively know this from statement 2 alone.
+Therefore, as Statement 1 suggests that a clue is associated with exactly one player but Statement 2 implies multiple clues could be tied to a single player, the multiplicity described seems to differ. However, the exact multiplicity in Statement 2 is unclear due to lack of specific information.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>If a player can disprove the hypothesis, that information is communicated only to the inquiring player.</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player can have hypothesis </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Statement 2 indicates that a player can disprove a hypothesis, which further implies that a player is associated with one or more hypotheses. However, the statement also adds that "that information is communicated only to the inquiring player". Here, it becomes uncertain whether each player is linked to a unique set of hypotheses, or whether all players can, in theory, disprove the same hypotheses but only the inquirer gets the feedback. 
+The former scenario would mean that each player is linked to many unique hypotheses, indicating a one-to-many relationship from player to hypothesis. The latter scenario, on the other hand, tells us that multiple players can be linked to the same hypotheses, indicating a many-to-many relationship.
+Since statement 2 does not specify either scenario, we do not have enough details to determine whether the multiplicity of the relationship between players and hypotheses differs from the multiplicity described in statement 1.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>The game's strategy is embodied in selecting questions to ask other players, selecting planet destinations, and efficiently deducing the correct murder scenario.</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>A player can have asks which are questions</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Statement 2 explains the strategy for the game wherein players have the role of selecting questions to ask other players. This suggests that there is an association between player and question as players select questions. However, it doesn't specifically establish whether a single player can have one or many questions - it merely states that players select questions. Given the vagueness of statement 2 regarding the multiplicity of this association, we cannot definitively say whether it matches the multiplicity in statement 1 (which clearly defines a player to have many questions).
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>As the players travel through the universe, they are permitted to ask questions about what information their fellow players possess.</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>A player can have asks which are questions</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests that a player asks questions as they progress through the universe. This implies there is an association between the player (as the actor asking the question) and the question (which is the action or behavior). However, statement 2 lacks specifics regarding how many questions a player can ask. 
+Statement 1 explicitly states that "a player can have asks which are questions" which is an indication of multiple questions (more than one question). Therefore, the multiplicity in statement 1 is 'many'.
+Considering these details, it seems that statement 2 implies the possibility of multiple questions. However, it does not clarify the exact number or frequency of questions, making a precise multiplicity from player to question unknown.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>The questions form a hypothesis for the murder circumstance and perpetrator, which the remaining players are invited to disprove with their evidence.</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>A player can have asks which are questions</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Statement 2 describes that the questions form a hypothesis for the murder circumstance and perpetrator, which the remaining players are invited to disprove with their evidence. This suggests questions have an association with all remaining players since all of them are invited to disprove the hypotheses.
+However, there is no specific mention of the exact multiplicity from player to question. There is an implication that it could be "many to many" (because many players are invited to disprove many questions) but it is not explicitly stated. 
+Therefore, we cannot clearly determine if the multiplicity differs from the one described in statement 1 which is "one to many" from player to question. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>A player whose token resides on one of four planets having wormhole connections to other planets may choose not to spin the spinner and take the wormhole directly to the other planet.</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player travels to planets </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Statement 2 states that one player’s token resides on one of four planets, and from that planet, the player may choose to travel directly to another planet via a wormhole connection. This implies that a singular instance of a player can be associated with one particular planet at a time (the one where the player's token resides), and also has the potential to be associated with another different planet (the one the player travels to via wormhole).
+However, it also separates the planets into two distinct types - those with wormhole connections, and those without. It is not explicitly stated whether a player can travel to many planets with wormhole connections, or only one at a time. Despite this, the ability for the player to move from one planet to another implies that at least a one-to-many association can exist between player and planets (even if only considering the planets with wormhole connections). 
+Although this suggests a multiplicity similar than that described in Statement 1, the mention of modifying conditions (i.e., the presence of wormhole connections) may impact the interpretation of the multiplicity, and without further context it is difficult to definitively state whether it is identical or not. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>A player may not re-visit the same planet on a single turn.</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A player travels to planets </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Statement 2 implies that a player can visit multiple planets, but he/she can't visit the same one twice during a single turn. This requirement tells us that within a single turn, a player can have many associations with instances of type "planet", but those associations must be unique within that turn. The player's association with each planet is therefore 1-to-1 during a turn.
+However, statement 1 seems to suggest a "one-to-many" relationship where a player can travel to many different planets without the restriction mentioned in statement 2. The multiplicity in statement 1 doesn't specify anything about the order or number of turns in which the planets are visited.
+Therefore, while both statements agree that a player (one instance) can travel to many (multiple instances) planets, they appear to disagree on the uniqueness requirement within a single turn. Statement 2 imposes an additional condition to the association not presented in statement 1.
+Conclusion: Yes, the multiplicity of statement 2 differs from the one described in statement 1.</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>A player wins the game by announcing their murder hypothesis, consisting of a planet, a perpetrator, and a murder weapon at any time during their turn, and having the server determine that the hypothesis is correct.</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>In statement 2, a game-winning scenario is described, where a player announces their solution (or "murder hypothesis") to a mystery. This hypothesis includes naming a certain planet. However, it is not stated that this planet can have associations with multiple other planets. The notation of a planet here appears more as an attribute of the murder hypothesis, rather than implying a set of associations or relationships to many other planets.
+Based on the given information, statement 2 does not specify a similar planet-to-planet relationship or multiplicity as described in statement 1. Therefore, the multiplicity (if any) from planet to planet in the context of statement 2 remains unclear or unspecified.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>The game is an intergalactic murder mystery, which emulates a board game scenario in which players spin a wheel to determine a randomly selected number of moves by which they travel through space to various planets.</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a game scenario where players move through space to various planets. So, there is an association between planets, as players can travel between them. However, the description in statement 2 doesn't indicate if one planet is associated with multiple others. We can infer that players can travel to multiple planets, but it's not clear whether each planet is necessarily connected to multiple others, or whether the nature of the game allows for indirect transfer from one planet to another through a sequence of moves.
+In contrast, Statement 1 expressly states that a planet is associated with many instances of other planets, indicating a one-to-many relationship.
+Considering that the detail in Statement 2 is ambiguous about multiplicity from planet to planet and doesn't specify a one-to-many relationship as Statement 1 does, the response would conclude:
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>The wormholes connect certain planets.</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Statement 2 specifies that wormholes connect "certain" planets. This suggests that not every planet is connected to every other planet through wormholes, which might imply a less "many" relationship between planets and suggests the possibility of either a one-to-many (one planet has wormholes to many others) or many-to-many (many planets have wormholes to many others) relationship, depending on the presence of additional context.
+However, the critical detail here is not specified; that is, whether one planet can have wormholes connecting to more than one other planet or not. If it can, then the multiplicity is many-to-many. If not, then the multiplicity is one-to-one. This lack of detail means that the multiplicity of statement 2 is not clear.
+Statement 1, in contrast, explicitly states an association with many instances of type planet meaning that a planet can have wormholes to many other planets. This describes a one-to-many relationship.
+Because the explicit multiplicity in statement 1 does not match the ambiguous multiplicity inferred from statement 2, we conclude that the multiplicities potentially defer between the two statements. 
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>To visit a planet, a player must enter the planet's atmosphere at one of the predefined entry points.</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Statement 2 seems to refer to the interaction between a player and a planet, stating that a player must enter a planet's atmosphere at one of the predefined entry points to visit that planet. There seems to be no direct association between planets mentioned in this statement. The multiplicity with respect to planets is not outlined explicitly in this context. Therefore, based on statement 2, we cannot determine the multiplicity from planet to planet.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>The game's strategy is embodied in selecting questions to ask other players, selecting planet destinations, and efficiently deducing the correct murder scenario.</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Statement 2 discusses the strategy of a game in which a player may select planet destinations. The language used in the statement, “selecting planet destinations,” suggests that a player can choose several planets, which implies the concept of one-to-many relationships. However, it does not explicitly mention the association among the planets themselves, i.e., unlike in statement 1, it does not clearly state any direct interaction between one planet and other planets. Therefore, determining the exact multiplicity from planet to planet in statement 2 becomes challenging. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Each planet has between one and three predefined atmospheric entry points.</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Statement 2 says - "Each planet has between one and three predefined atmospheric entry points." This statement does not talk or infer about any associations of one planet with another planet. It is essentially talking about certain characteristics or features (atmospheric entry points) of a single planet. An analogy can be drawn to a single person having between one to two phone numbers - it does not tell anything about the relationship of the person with others.
+Therefore, it's not possible to determine the multiplicity from planet to planet from this statement.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>The player is considered to be on the planet as soon as the planet's atmosphere has been entered.</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Statement 2 implies a single association between a player and a planet but does not explicitly mention any direct multiplicity between planets. Rather, it focuses on the relationship between a player and a planet indicating a one-to-one association. 
+On the other hand, statement 1 states a multiplicity between multiple instances of a planet, indicating the possibility of multiple associations. 
+Therefore, it can be concluded that the multiplicity in statement 2, if it exists, between the planet and the planet is different from the one described in the statement 1. 
+Conclusion: Yes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>The player can enter the planet's atmosphere in a different number of moves.</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Statement 2 does not provide a direct relationship or association between two planets. Instead, it talks about the association between a player and a planet focusing on how the player can enter the planet's atmosphere which is a different type of relationship.
+This statement does not provide an equivalent multiplicity to Statement 1’s “a planet has wormhole to planets,” which describes a multiples-to-multiple relationship between planets. At best, statement 2 describes a one-to-many relationship between a player and the moves they can make to enter a planet's atmosphere. 
+However, the nature of relationships in the two statements are considerably different, with the first describing a relationship between two planets and the second between a player and a planet. This difference makes it difficult to accurately compare the multiplicities.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>A player may not re-visit the same planet on a single turn.</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Statement 2 suggests a rule for a player's movement rather than describing the relationship between planets. Most importantly, it specifies that a player may not visit the same planet twice in one turn. However, this does not really elaborate on or describe the nature of connectivity or multiplicity from planet to planet. The ability of a player not to return to a planet on the same turn may be governed by game rules instead of any inherent relationships or associations between planets themselves. 
+Therefore, statement 2 does not provide enough details to determine the multiplicity from planet to planet.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>These entry points are graphically depicted on the game as a diagonal line off a square on the board leading into a planet's atmosphere.</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Analyzing statement 2, there is no clear indication of the multiplicity between a planet and other planets. The statement explains about entry points leading into a planet's atmosphere. However, it does not disclose how many planets can be associated with each entry point, or if a planet can be associated with many entry points from various planets. Given the limited information in statement 2, it is difficult to establish the level of multiplicity in the relation between one planet and another.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>The objective of player movement throughout the universe is to investigate specific planets to determine if that was the murder site.</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A planet haves warmhole to planets </t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>In statement 2, we see a single instance of a planet being investigated to be the murder site. So, the multiplicity, in this case, would seem to be from one planet to another single planet. Compared to statement 1, where a planet could be associated with many planets, this is a different multiplicity, assuming that investigation of a specific planet means the association with that specific planet alone in the context of this particular task.
+Conclusion: Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>A player wins the game by announcing their murder hypothesis, consisting of a planet, a perpetrator, and a murder weapon at any time during their turn, and having the server determine that the hypothesis is correct.</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a game in which a player wins by announcing their "murder hypothesis". This murder hypothesis is said to consist of a planet, a perpetrator, and a murder weapon. Implicit in this statement is the idea that there is only one of each of these components in the murder hypothesis. That is, each hypothesis is associated with a single planet, a single perpetrator, and a single weapon.
+This means the multiplicity from hypothesis to planet in statement 2 is "one", just like in statement 1. So, it doesn't differ from the multiplicity outlined in statement 1.
+Conclusion: No</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>The game is an intergalactic murder mystery, which emulates a board game scenario in which players spin a wheel to determine a randomly selected number of moves by which they travel through space to various planets.</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Statement 2 seems to describe a game scenario where players can travel to various planets. However, there's no clear information about how a hypothesis would be associated with these planets within the context of the game. It's only stated that there are various planets involved in the game scenario and not the specific relationship between a hypothesis and these planets.
+To determine the multiplicity from hypothesis to planet based on statement 2, we need explicit information about how a hypothesis relates to the planets in this game context, which is missing. Thus, there's insufficient detail in statement 2 to firmly establish an association or determine the multiplicity of the relationship from hypothesis to the planet.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>The wormholes connect certain planets.</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Statement 2 mentions that 'wormholes connect certain planets'. However, it does not explicitly mention any association between a hypothesis and a planet. Even if there was a hidden association, it does not provide any clear information on the multiplicity of that association.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>To visit a planet, a player must enter the planet's atmosphere at one of the predefined entry points.</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Statement 2 describes the requirements for a player to visit a planet, but it does not comment on the relationship between a hypothesis and a planet. There isn't any information provided that suggests a hypothesis is associated with multiple planets, or the inverse. Since the association between hypothesis and planet isn't specified in statement 2, it's unclear if the multiplicity differs from that defined in statement 1.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>The game's strategy is embodied in selecting questions to ask other players, selecting planet destinations, and efficiently deducing the correct murder scenario.</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Statement 2 does not provide a clear association between a hypothesis and a planet. It only specifies that in the game's strategy, players choose planet destinations among other actions. It doesn't explicitly say that these chosen planets are linked to a hypothesis. Moreover, it does not indicate whether a hypothesis is associated with one or more planets. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Each planet has between one and three predefined atmospheric entry points.</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>The second statement says that "Each planet has between one and three predefined atmospheric entry points." Here, the entity being talked about is 'planet' and not hypothesis. Therefore, it doesn't directly provide information about multiplicity between the hypothesis and the planet. 
+However, if we consider that each atmosphere entry point may require a separate hypothesis or all require the same hypothesis, there could be a multiplicity change from 1:1 to be 1:1-3. This interpretation assumes that the process of defining each atmospheric entry point could be an independent hypothesis. Still, this is not explicitly stated in the provided information.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>The player is considered to be on the planet as soon as the planet's atmosphere has been entered.</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Statement 2 describes that a player is associated with a planet once they enter the atmosphere of such planet. However, it does not provide any information about the association or multiplicity between a hypothesis and a planet. It does not state if the hypothesis is connected to this action or occurrence. 
+Therefore, based on the information in statement 2, we cannot determine the multiplicity between hypothesis and planet, nor can we determine if there is any change in multiplicity from statement 1.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>The planets, Linuta and Verlute, have a wormhole connecting each other, as do Earth and Evilon.</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>The second statement provides information about the connectivity between different planets, specifying that each pair of two named planets is connected by a wormhole. However, this statement does not provide direct information about any association between a hypothesis and a planet.
+In the first statement, there is a specific mention that a hypothesis is associated with exactly one planet. If we are to imply an association from the second statement, there is none stated explicitly. If a hypothesis were associated with the existence of these wormholes, it would need to be associated with the pair of planets making each wormhole for it to exist, which could imply a hypothesis potentially being associated with more than one planet, but this is not explicitly stated.
+Therefore, based on the available information in the second statement, we cannot specifically determine the multiplicity from hypothesis to planet.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>The player can enter the planet's atmosphere in a different number of moves.</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>In the first statement, it mentioned that a hypothesis has exactly one planet. This implies a one-to-one correspondence between a hypothesis and a planet.
+However, in the second statement, while it does involve the planet, it does not provide clear information about how the player's actions (entering the planet's atmosphere in a different number of moves) connect to the hypothesis. It's possible that different hypotheses might interact with the process of entering the planet's atmosphere, but without explicit details indicating such, we can't confirm the association or determine the multiplicity between the hypothesis and the planet.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>A player visits a planet by making legal moves on the board until a cell adjacent to an atmosphere entry point is reached.</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Statement 2 describes the process of a player’s movement towards a planet within a game setup. However, it doesn't provide any information about the relationship between a hypothesis and a planet. Therefore, we cannot determine any multiplicity from hypothesis to planet based on statement 2. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>A player may not re-visit the same planet on a single turn.</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Statement 2 discusses a different context - it places a condition on the player's action (not being able to revisit the same planet within a single turn) rather than addressing the relationship between a hypothesis and a planet. The multiplicity of association discussed applies to different things - 'player' to 'planet', not 'hypothesis' to 'planet'. 
+Thus, we cannot directly derive or analyze the multiplicity from 'hypothesis' to 'planet' based on statement 2.
+Conclusion: Not Sure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>These entry points are graphically depicted on the game as a diagonal line off a square on the board leading into a planet's atmosphere.</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Statement 2 talks about entry points graphically depicted on a game leading into a planet's atmosphere. However, it does not mention any relationship between a hypothesis and a planet. Therefore, there is no way we could determine the multiplicity from hypothesis to planet from statement 2. 
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>A player whose token resides on one of four planets having wormhole connections to other planets may choose not to spin the spinner and take the wormhole directly to the other planet.</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>A hypothesis has a planet</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Statement 2 describes a scenario where a player's token resides on one of four planets with wormhole connections to other planets. However, it does not provide any explicit connection or association between a hypothesis and a planet. Therefore, determining multiplicity of a hypothesis to a planet from this statement alone cannot be done with any certainty.
+Conclusion: Not Sure</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>